<commit_message>
FLOBO-2021 first work day
</commit_message>
<xml_diff>
--- a/text/Statistik.xlsx
+++ b/text/Statistik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korme\Documents\Feuerwehr\Flobo\Florianibote2021\text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feuerwehr Lengenfeld\Documents\Flobo\2021\Florianibote2021\text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9A9EA-C295-4361-A332-14638395B045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93B4383-6AEE-4541-971A-16379BBAE731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Einsätze" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Testen!$K$7:$K$9</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Testen!$L$7:$L$9</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Testen!$K$7:$K$9</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Testen!$L$7:$L$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,9 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -3171,7 +3171,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>117 Übungen und Schulungen</a:t>
+                <a:t>79 Übungen und Schulungen</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -3455,7 +3455,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t>4760 Stunden</a:t>
+              <a:t>6846 Stunden</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="de-AT" sz="1400" baseline="0">
@@ -3480,7 +3480,7 @@
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t>119 000 Euro Arbeitsleistung</a:t>
+              <a:t>171,150 Euro Arbeitsleistung</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -3804,7 +3804,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>52 technische</a:t>
+                <a:t>91 technische</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="de-AT" sz="1400" baseline="0">
@@ -3926,20 +3926,12 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="de-AT" sz="1400">
-                  <a:solidFill>
-                    <a:srgbClr val="C00000"/>
-                  </a:solidFill>
-                </a:rPr>
-                <a:t>4</a:t>
-              </a:r>
-              <a:r>
                 <a:rPr lang="de-AT" sz="1400" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="C00000"/>
                   </a:solidFill>
                 </a:rPr>
-                <a:t> Brandeinsätze</a:t>
+                <a:t>5 Brandeinsätze</a:t>
               </a:r>
               <a:endParaRPr lang="de-AT" sz="1400">
                 <a:solidFill>
@@ -4448,16 +4440,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>33618</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>618725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>605119</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>112059</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>537083</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>98452</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4472,79 +4464,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33618" y="89647"/>
-          <a:ext cx="5860677" cy="3451412"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="28575" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-AT" sz="1100">
-            <a:ln w="28575">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>181535</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>81296</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>68917</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>120464</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="76" name="TextBox 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A171DFAB-529B-42BE-8D3F-037DBD4FAD6E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6753785" y="3700796"/>
-          <a:ext cx="4487957" cy="2706168"/>
+          <a:off x="5843868" y="1600040"/>
+          <a:ext cx="5796644" cy="3451412"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4591,15 +4512,86 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>24655</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>170329</xdr:rowOff>
+      <xdr:colOff>59071</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>81296</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>599596</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
+      <xdr:rowOff>120464</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="TextBox 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A171DFAB-529B-42BE-8D3F-037DBD4FAD6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="59071" y="6558296"/>
+          <a:ext cx="4459382" cy="2706168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-AT" sz="1100">
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>174334</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>143115</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>160885</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>152081</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4614,8 +4606,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24655" y="6266329"/>
-          <a:ext cx="4614580" cy="3056966"/>
+          <a:off x="4093191" y="5286615"/>
+          <a:ext cx="4558551" cy="3056966"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5520,7 +5512,7 @@
   <dimension ref="K7:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5538,7 +5530,7 @@
         <v>12</v>
       </c>
       <c r="L8">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="11:12" x14ac:dyDescent="0.25">

</xml_diff>